<commit_message>
change names of abvMonth -> abrvMonth and distanceIsoWeek -> countIsoWeek
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -1,20 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gedeonz/Dev/R Sources/STRAP Common Tasks/sources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D911E4-F5AD-3541-9229-2E0C1B2C017F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="740" windowWidth="28800" windowHeight="14920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="T2" sheetId="2" r:id="rId1"/>
-    <sheet name="T3" sheetId="17" r:id="rId2"/>
+    <sheet name="T2" sheetId="2" state="visible" r:id="rId1"/>
+    <sheet name="T3" sheetId="17" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>n</t>
   </si>
@@ -209,7 +202,7 @@
     <t>Miguel Servet Hospital, Zaragoza</t>
   </si>
   <si>
-    <t/>
+    <t>NA</t>
   </si>
   <si>
     <t>test xlsx</t>
@@ -258,6 +251,36 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
   </si>
 </sst>
 </file>
@@ -267,7 +290,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,45 +303,26 @@
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color rgb="FF65B32E"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <b/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
       <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -329,7 +333,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -350,10 +354,38 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -363,204 +395,52 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -871,619 +751,622 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="true" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="1" max="1" width="41.5" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="12.5" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="10.5" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16" thickBot="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" ht="16" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-    </row>
-    <row r="2" spans="1:21" ht="39.75" customHeight="1" thickBot="1">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+    </row>
+    <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="5" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="5" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="5" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="6"/>
-    </row>
-    <row r="3" spans="1:21" ht="16" thickBot="1">
-      <c r="A3" s="2"/>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="U2" s="9"/>
+    </row>
+    <row r="3" ht="16" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" t="n">
+        <v>67</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.744444444444444</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-    </row>
-    <row r="4" spans="1:21" ht="16" thickBot="1">
-      <c r="A4" s="9" t="s">
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+    </row>
+    <row r="4" ht="16" customHeight="1">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="3" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="11">
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11">
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="11">
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="11">
+      <c r="K4" s="2"/>
+      <c r="L4" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="11">
+      <c r="M4" s="2"/>
+      <c r="N4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="11">
+      <c r="O4" s="2"/>
+      <c r="P4" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="11">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="11">
+      <c r="S4" s="2"/>
+      <c r="T4" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="12"/>
-    </row>
-    <row r="5" spans="1:21" ht="16" thickBot="1">
-      <c r="A5" s="9" t="s">
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" ht="16" customHeight="1">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="3" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="4" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="3" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="4" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="3" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="4" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="3" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="4" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="3" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="4" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="13">
-        <v>0</v>
-      </c>
-      <c r="O5" s="18">
-        <v>0</v>
-      </c>
-      <c r="P5" s="13">
+      <c r="N5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="Q5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="18">
+      <c r="S5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="16" thickBot="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" ht="16" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="3" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="4" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="4" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="4" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="4" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="4" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="14">
-        <v>0</v>
-      </c>
-      <c r="M6" s="18">
-        <v>0</v>
-      </c>
-      <c r="N6" s="14">
+      <c r="L6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>0</v>
-      </c>
-      <c r="R6" s="14">
-        <v>0</v>
-      </c>
-      <c r="S6" s="18">
-        <v>0</v>
-      </c>
-      <c r="T6" s="14">
-        <v>0</v>
-      </c>
-      <c r="U6" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="16" thickBot="1">
-      <c r="A7" s="9" t="s">
+      <c r="P6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="3" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="4" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="15">
-        <v>0</v>
-      </c>
-      <c r="E7" s="19">
-        <v>0</v>
-      </c>
-      <c r="F7" s="15">
-        <v>0</v>
-      </c>
-      <c r="G7" s="19">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15">
-        <v>0</v>
-      </c>
-      <c r="I7" s="19">
-        <v>0</v>
-      </c>
-      <c r="J7" s="15">
-        <v>0</v>
-      </c>
-      <c r="K7" s="19">
-        <v>0</v>
-      </c>
-      <c r="L7" s="15">
-        <v>0</v>
-      </c>
-      <c r="M7" s="19" t="e">
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="19" t="e">
+      <c r="P7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="15">
-        <v>0</v>
-      </c>
-      <c r="S7" s="19" t="e">
+      <c r="R7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="15">
-        <v>0</v>
-      </c>
-      <c r="U7" s="19" t="e">
+      <c r="T7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="16" thickBot="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="10"/>
-    </row>
-    <row r="9" spans="1:21" ht="16" thickBot="1">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="3" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="4" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="17">
-        <v>0</v>
-      </c>
-      <c r="E9" s="19">
-        <v>0</v>
-      </c>
-      <c r="F9" s="17">
-        <v>0</v>
-      </c>
-      <c r="G9" s="19">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17">
-        <v>0</v>
-      </c>
-      <c r="I9" s="19">
-        <v>0</v>
-      </c>
-      <c r="J9" s="17">
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="17">
-        <v>0</v>
-      </c>
-      <c r="M9" s="19" t="e">
+      <c r="L9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="17">
-        <v>0</v>
-      </c>
-      <c r="O9" s="19">
-        <v>0</v>
-      </c>
-      <c r="P9" s="17">
+      <c r="N9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="19" t="e">
+      <c r="Q9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="17">
+      <c r="R9" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="19" t="e">
+      <c r="S9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="17">
-        <v>0</v>
-      </c>
-      <c r="U9" s="19" t="e">
+      <c r="T9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16" thickBot="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="3" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="2" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="16">
-        <v>0</v>
-      </c>
-      <c r="F10" s="14">
-        <v>0</v>
-      </c>
-      <c r="G10" s="16">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14">
-        <v>0</v>
-      </c>
-      <c r="I10" s="16">
-        <v>0</v>
-      </c>
-      <c r="J10" s="14">
-        <v>0</v>
-      </c>
-      <c r="K10" s="16">
-        <v>0</v>
-      </c>
-      <c r="L10" s="14">
-        <v>0</v>
-      </c>
-      <c r="M10" s="16" t="e">
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="14">
-        <v>0</v>
-      </c>
-      <c r="O10" s="16">
-        <v>0</v>
-      </c>
-      <c r="P10" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="16" t="e">
+      <c r="N10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="14">
-        <v>0</v>
-      </c>
-      <c r="S10" s="16" t="e">
+      <c r="R10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="14">
-        <v>0</v>
-      </c>
-      <c r="U10" s="16" t="e">
+      <c r="T10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="7" t="s">
+    <row r="11">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="8" t="s">
+    <row r="12">
+      <c r="A12" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="8" t="s">
+    <row r="13">
+      <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="8" t="s">
+    <row r="14">
+      <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="8" t="s">
+    <row r="15">
+      <c r="A15" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="7"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="7"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="7"/>
+    <row r="16">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1CCA03-CDAA-2342-A111-C5F7B56D790A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6"/>
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>47</v>
+      </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
         <v>40</v>
@@ -1491,50 +1374,59 @@
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="K7" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="K8" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
       <c r="J9" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="K9" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="L10" t="n">
+        <v>5</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
addition of simple cross table creating function : crosstab
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>n</t>
   </si>
@@ -282,6 +282,9 @@
   <si>
     <t xml:space="preserve">2</t>
   </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
 </sst>
 </file>
 
@@ -290,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,27 +305,40 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF65B32E"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
       <b/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
-      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF65B32E"/>
+      <name val="Tahoma"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <i/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -356,6 +372,9 @@
       </bottom>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -364,9 +383,6 @@
       </bottom>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -400,27 +416,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -429,15 +454,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -802,525 +821,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="8" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="8" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="9"/>
+      <c r="U2" s="12"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="6" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="n">
+      <c r="E4" s="5"/>
+      <c r="F4" s="6" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="n">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3" t="n">
+      <c r="I4" s="5"/>
+      <c r="J4" s="6" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3" t="n">
+      <c r="K4" s="5"/>
+      <c r="L4" s="6" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3" t="n">
+      <c r="M4" s="5"/>
+      <c r="N4" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3" t="n">
+      <c r="O4" s="5"/>
+      <c r="P4" s="6" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="3" t="n">
+      <c r="Q4" s="5"/>
+      <c r="R4" s="6" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="3" t="n">
+      <c r="S4" s="5"/>
+      <c r="T4" s="6" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="2"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="6" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="7" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="6" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="7" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="7" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="6" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="7" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="6" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="7" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="6" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3" t="n">
+      <c r="N5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="4" t="n">
+      <c r="Q5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="3" t="n">
+      <c r="R5" s="6" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="4" t="n">
+      <c r="S5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="3" t="n">
+      <c r="T5" s="6" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="4" t="n">
+      <c r="U5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="6" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="7" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="7" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="7" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="7" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="7" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3" t="n">
+      <c r="L6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="4" t="n">
+      <c r="O6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="4" t="n">
+      <c r="P6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="6" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="7" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4" t="e">
+      <c r="D7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="3" t="n">
+      <c r="N7" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="4" t="n">
+      <c r="O7" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4" t="e">
+      <c r="P7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4" t="e">
+      <c r="R7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="4" t="e">
+      <c r="T7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="7" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="6" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C9" s="7" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3" t="n">
+      <c r="D9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="4" t="n">
+      <c r="K9" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4" t="e">
+      <c r="L9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="N9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="4" t="e">
+      <c r="Q9" s="7" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="3" t="n">
+      <c r="R9" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="4" t="e">
+      <c r="S9" s="7" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="4" t="e">
+      <c r="T9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="7" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="6" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="5" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2" t="e">
+      <c r="D10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2" t="e">
+      <c r="N10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="2" t="e">
+      <c r="R10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="2" t="e">
+      <c r="T10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="5" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="10"/>
+      <c r="A17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="15" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="10"/>
+      <c r="A19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
upload of lastDateMonth function
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -308,6 +308,17 @@
       <b/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <i/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
@@ -328,17 +339,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00FF00"/>
-      <name val="Calibri"/>
-      <i/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -367,17 +367,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -412,6 +401,17 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -421,41 +421,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -785,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -821,533 +821,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="11" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="11" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="11" t="s">
+      <c r="Q2" s="4"/>
+      <c r="R2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="11" t="s">
+      <c r="S2" s="4"/>
+      <c r="T2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="12"/>
+      <c r="U2" s="4"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="13"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="11" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="n">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="n">
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6" t="n">
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6" t="n">
+      <c r="I4" s="10"/>
+      <c r="J4" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6" t="n">
+      <c r="K4" s="10"/>
+      <c r="L4" s="11" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6" t="n">
+      <c r="M4" s="10"/>
+      <c r="N4" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6" t="n">
+      <c r="O4" s="10"/>
+      <c r="P4" s="11" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="6" t="n">
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="6" t="n">
+      <c r="S4" s="10"/>
+      <c r="T4" s="11" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="5"/>
+      <c r="U4" s="10"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="11" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="12" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="11" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="12" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="11" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="12" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="11" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="12" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="11" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="7" t="n">
+      <c r="K5" s="12" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="6" t="n">
+      <c r="L5" s="11" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="7" t="n">
+      <c r="M5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="n">
+      <c r="N5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="7" t="n">
+      <c r="Q5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="6" t="n">
+      <c r="R5" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="7" t="n">
+      <c r="S5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="6" t="n">
+      <c r="T5" s="11" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="U5" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="11" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="12" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="12" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="12" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="12" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="7" t="n">
+      <c r="K6" s="12" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6" t="n">
+      <c r="L6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="7" t="n">
+      <c r="O6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="7" t="n">
+      <c r="P6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="11" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="12" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7" t="e">
+      <c r="D7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="6" t="n">
+      <c r="N7" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="7" t="n">
+      <c r="O7" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7" t="e">
+      <c r="P7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="7" t="e">
+      <c r="R7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="7" t="e">
+      <c r="T7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="10"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="11" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="12" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6" t="n">
+      <c r="D9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="7" t="e">
+      <c r="L9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6" t="n">
+      <c r="N9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="7" t="e">
+      <c r="Q9" s="12" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="6" t="n">
+      <c r="R9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="7" t="e">
+      <c r="S9" s="12" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="7" t="e">
+      <c r="T9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="12" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="11" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="10" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5" t="e">
+      <c r="D10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5" t="e">
+      <c r="N10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5" t="e">
+      <c r="R10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5" t="e">
+      <c r="T10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="10" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
+      <c r="A16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="15" t="n">
+      <c r="C17" s="6" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
+      <c r="A19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Small change for managing missing values in table Help updated to current version
Docs updated accordingly
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -308,6 +308,17 @@
       <b/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <i/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
@@ -328,17 +339,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00FF00"/>
-      <name val="Calibri"/>
-      <i/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -367,17 +367,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -412,6 +401,17 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -421,41 +421,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -785,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -821,533 +821,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="11" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="11" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="11" t="s">
+      <c r="Q2" s="4"/>
+      <c r="R2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="11" t="s">
+      <c r="S2" s="4"/>
+      <c r="T2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="12"/>
+      <c r="U2" s="4"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="13"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="11" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="n">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="n">
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6" t="n">
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6" t="n">
+      <c r="I4" s="10"/>
+      <c r="J4" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6" t="n">
+      <c r="K4" s="10"/>
+      <c r="L4" s="11" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6" t="n">
+      <c r="M4" s="10"/>
+      <c r="N4" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6" t="n">
+      <c r="O4" s="10"/>
+      <c r="P4" s="11" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="6" t="n">
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="6" t="n">
+      <c r="S4" s="10"/>
+      <c r="T4" s="11" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="5"/>
+      <c r="U4" s="10"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="11" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="12" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="11" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="12" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="11" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="12" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="11" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="12" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="11" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="7" t="n">
+      <c r="K5" s="12" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="6" t="n">
+      <c r="L5" s="11" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="7" t="n">
+      <c r="M5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="n">
+      <c r="N5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="7" t="n">
+      <c r="Q5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="6" t="n">
+      <c r="R5" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="7" t="n">
+      <c r="S5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="6" t="n">
+      <c r="T5" s="11" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="U5" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="11" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="12" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="12" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="12" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="12" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="7" t="n">
+      <c r="K6" s="12" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6" t="n">
+      <c r="L6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="7" t="n">
+      <c r="O6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="7" t="n">
+      <c r="P6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="11" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="12" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7" t="e">
+      <c r="D7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="6" t="n">
+      <c r="N7" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="7" t="n">
+      <c r="O7" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7" t="e">
+      <c r="P7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="7" t="e">
+      <c r="R7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="7" t="e">
+      <c r="T7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="10"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="11" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="12" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6" t="n">
+      <c r="D9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="7" t="e">
+      <c r="L9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6" t="n">
+      <c r="N9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="7" t="e">
+      <c r="Q9" s="12" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="6" t="n">
+      <c r="R9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="7" t="e">
+      <c r="S9" s="12" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="7" t="e">
+      <c r="T9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="12" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="11" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="10" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5" t="e">
+      <c r="D10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5" t="e">
+      <c r="N10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5" t="e">
+      <c r="R10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5" t="e">
+      <c r="T10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="10" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
+      <c r="A16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="15" t="n">
+      <c r="C17" s="6" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
+      <c r="A19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
changed by test... to be solved
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -308,6 +308,17 @@
       <b/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF65B32E"/>
+      <name val="Tahoma"/>
+      <b/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF00FF00"/>
       <name val="Calibri"/>
@@ -322,17 +333,6 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF65B32E"/>
-      <name val="Tahoma"/>
-      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -383,6 +383,17 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -401,17 +412,6 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -421,40 +421,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -785,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -821,533 +821,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="3" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="3" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="3" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="4"/>
+      <c r="U2" s="9"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="13"/>
+      <c r="A3" s="5"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="3" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="n">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11" t="n">
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="n">
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11" t="n">
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11" t="n">
+      <c r="K4" s="2"/>
+      <c r="L4" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11" t="n">
+      <c r="M4" s="2"/>
+      <c r="N4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11" t="n">
+      <c r="O4" s="2"/>
+      <c r="P4" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="11" t="n">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="10"/>
-      <c r="T4" s="11" t="n">
+      <c r="S4" s="2"/>
+      <c r="T4" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="10"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="3" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="4" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="3" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="4" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="11" t="n">
+      <c r="F5" s="3" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="12" t="n">
+      <c r="G5" s="4" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="11" t="n">
+      <c r="H5" s="3" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="I5" s="4" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="11" t="n">
+      <c r="J5" s="3" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="12" t="n">
+      <c r="K5" s="4" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="11" t="n">
+      <c r="L5" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="M5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="11" t="n">
+      <c r="N5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="12" t="n">
+      <c r="Q5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="11" t="n">
+      <c r="R5" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="12" t="n">
+      <c r="S5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="11" t="n">
+      <c r="T5" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="12" t="n">
+      <c r="U5" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="3" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="4" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="12" t="n">
+      <c r="E6" s="4" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="11" t="n">
+      <c r="F6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="12" t="n">
+      <c r="G6" s="4" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="11" t="n">
+      <c r="H6" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="12" t="n">
+      <c r="I6" s="4" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="11" t="n">
+      <c r="J6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="12" t="n">
+      <c r="K6" s="4" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="11" t="n">
+      <c r="L6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="12" t="n">
+      <c r="O6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="12" t="n">
+      <c r="P6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="3" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="4" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="12" t="e">
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="11" t="n">
+      <c r="N7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="12" t="n">
+      <c r="O7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="12" t="e">
+      <c r="P7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="12" t="e">
+      <c r="R7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="12" t="e">
+      <c r="T7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="10"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="2"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="3" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="4" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11" t="n">
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="12" t="n">
+      <c r="K9" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="12" t="e">
+      <c r="L9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="11" t="n">
+      <c r="N9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="12" t="e">
+      <c r="Q9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="11" t="n">
+      <c r="R9" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="12" t="e">
+      <c r="S9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="12" t="e">
+      <c r="T9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="3" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="2" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="10" t="e">
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10" t="e">
+      <c r="N10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="10" t="e">
+      <c r="R10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="10" t="e">
+      <c r="T10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
+      <c r="A16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="11" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
+      <c r="A19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
addSep return a true string, paste0 is used to avoid space (if could be added to sep)
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>n</t>
   </si>
@@ -282,6 +282,9 @@
   <si>
     <t xml:space="preserve">2</t>
   </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
 </sst>
 </file>
 
@@ -290,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,27 +305,40 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF65B32E"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
       <b/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
-      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF65B32E"/>
+      <name val="Tahoma"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <i/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -356,6 +372,9 @@
       </bottom>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -364,9 +383,6 @@
       </bottom>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -400,27 +416,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -429,15 +454,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -802,525 +821,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="8" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="8" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="9"/>
+      <c r="U2" s="12"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="5"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="6" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="n">
+      <c r="E4" s="5"/>
+      <c r="F4" s="6" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="n">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3" t="n">
+      <c r="I4" s="5"/>
+      <c r="J4" s="6" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3" t="n">
+      <c r="K4" s="5"/>
+      <c r="L4" s="6" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3" t="n">
+      <c r="M4" s="5"/>
+      <c r="N4" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3" t="n">
+      <c r="O4" s="5"/>
+      <c r="P4" s="6" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="3" t="n">
+      <c r="Q4" s="5"/>
+      <c r="R4" s="6" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="3" t="n">
+      <c r="S4" s="5"/>
+      <c r="T4" s="6" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="2"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="6" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="7" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="6" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="7" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="7" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="6" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="7" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="6" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="7" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="6" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3" t="n">
+      <c r="N5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="4" t="n">
+      <c r="Q5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="3" t="n">
+      <c r="R5" s="6" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="4" t="n">
+      <c r="S5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="3" t="n">
+      <c r="T5" s="6" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="4" t="n">
+      <c r="U5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="6" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="7" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="7" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="7" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="7" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="7" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3" t="n">
+      <c r="L6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="4" t="n">
+      <c r="O6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="4" t="n">
+      <c r="P6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="6" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="7" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4" t="e">
+      <c r="D7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="3" t="n">
+      <c r="N7" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="4" t="n">
+      <c r="O7" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4" t="e">
+      <c r="P7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4" t="e">
+      <c r="R7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="4" t="e">
+      <c r="T7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="7" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="6" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C9" s="7" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3" t="n">
+      <c r="D9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="4" t="n">
+      <c r="K9" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4" t="e">
+      <c r="L9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="N9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="4" t="e">
+      <c r="Q9" s="7" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="3" t="n">
+      <c r="R9" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="4" t="e">
+      <c r="S9" s="7" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="4" t="e">
+      <c r="T9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="7" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="6" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="5" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2" t="e">
+      <c r="D10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2" t="e">
+      <c r="N10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="2" t="e">
+      <c r="R10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="2" t="e">
+      <c r="T10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="5" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="10"/>
+      <c r="A17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="15" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="10"/>
+      <c r="A19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Keyring function have been atomised for a smaller granularity. Each function does only one thing without user input. Function has been regrouped into the keyring.R script Keyring use has been totaly restructured to avoid creating "keyring" (keyring are container for multiple key) and to create secret keys in the default container instead. Default container is unlocked by the user session automaticaly Tests has been added
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -308,6 +308,17 @@
       <b/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <i/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
@@ -328,17 +339,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00FF00"/>
-      <name val="Calibri"/>
-      <i/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -367,17 +367,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -412,6 +401,17 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -421,41 +421,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -785,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -821,533 +821,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="11" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="11" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="11" t="s">
+      <c r="Q2" s="4"/>
+      <c r="R2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="11" t="s">
+      <c r="S2" s="4"/>
+      <c r="T2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="12"/>
+      <c r="U2" s="4"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="13"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="11" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="n">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="n">
+      <c r="E4" s="10"/>
+      <c r="F4" s="11" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6" t="n">
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6" t="n">
+      <c r="I4" s="10"/>
+      <c r="J4" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6" t="n">
+      <c r="K4" s="10"/>
+      <c r="L4" s="11" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6" t="n">
+      <c r="M4" s="10"/>
+      <c r="N4" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6" t="n">
+      <c r="O4" s="10"/>
+      <c r="P4" s="11" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="6" t="n">
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="6" t="n">
+      <c r="S4" s="10"/>
+      <c r="T4" s="11" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="5"/>
+      <c r="U4" s="10"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="11" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="12" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="11" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="12" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="11" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="12" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="11" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="12" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="11" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="7" t="n">
+      <c r="K5" s="12" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="6" t="n">
+      <c r="L5" s="11" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="7" t="n">
+      <c r="M5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="n">
+      <c r="N5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="7" t="n">
+      <c r="Q5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="6" t="n">
+      <c r="R5" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="7" t="n">
+      <c r="S5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="6" t="n">
+      <c r="T5" s="11" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="U5" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="11" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="12" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="12" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="12" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="12" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="7" t="n">
+      <c r="K6" s="12" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6" t="n">
+      <c r="L6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="7" t="n">
+      <c r="O6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="7" t="n">
+      <c r="P6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="11" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="12" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7" t="e">
+      <c r="D7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="6" t="n">
+      <c r="N7" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="7" t="n">
+      <c r="O7" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7" t="e">
+      <c r="P7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="7" t="e">
+      <c r="R7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="7" t="e">
+      <c r="T7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="10"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="11" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="12" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6" t="n">
+      <c r="D9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="7" t="e">
+      <c r="L9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6" t="n">
+      <c r="N9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="7" t="e">
+      <c r="Q9" s="12" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="6" t="n">
+      <c r="R9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="7" t="e">
+      <c r="S9" s="12" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="7" t="e">
+      <c r="T9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="12" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="11" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="10" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5" t="e">
+      <c r="D10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5" t="e">
+      <c r="N10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5" t="e">
+      <c r="R10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5" t="e">
+      <c r="T10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="10" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
+      <c r="A16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="15" t="n">
+      <c r="C17" s="6" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
+      <c r="A19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Conflict resoultion part 2
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -308,6 +308,17 @@
       <b/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF65B32E"/>
+      <name val="Tahoma"/>
+      <b/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF00FF00"/>
       <name val="Calibri"/>
@@ -322,17 +333,6 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF65B32E"/>
-      <name val="Tahoma"/>
-      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -383,6 +383,17 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -401,17 +412,6 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -421,40 +421,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -472,6 +472,41 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">1</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">19</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="6400800" cy="3657600"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="1" name="Picture 1"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -785,31 +820,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -821,533 +856,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="3" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="3" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="3" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="4"/>
+      <c r="U2" s="9"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="13"/>
+      <c r="A3" s="5"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="3" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="n">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11" t="n">
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="n">
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11" t="n">
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11" t="n">
+      <c r="K4" s="2"/>
+      <c r="L4" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11" t="n">
+      <c r="M4" s="2"/>
+      <c r="N4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11" t="n">
+      <c r="O4" s="2"/>
+      <c r="P4" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="11" t="n">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="10"/>
-      <c r="T4" s="11" t="n">
+      <c r="S4" s="2"/>
+      <c r="T4" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="10"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="3" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="4" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="3" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="4" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="11" t="n">
+      <c r="F5" s="3" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="12" t="n">
+      <c r="G5" s="4" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="11" t="n">
+      <c r="H5" s="3" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="I5" s="4" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="11" t="n">
+      <c r="J5" s="3" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="12" t="n">
+      <c r="K5" s="4" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="11" t="n">
+      <c r="L5" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="M5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="11" t="n">
+      <c r="N5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="12" t="n">
+      <c r="Q5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="11" t="n">
+      <c r="R5" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="12" t="n">
+      <c r="S5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="11" t="n">
+      <c r="T5" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="12" t="n">
+      <c r="U5" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="3" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="4" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="12" t="n">
+      <c r="E6" s="4" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="11" t="n">
+      <c r="F6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="12" t="n">
+      <c r="G6" s="4" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="11" t="n">
+      <c r="H6" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="12" t="n">
+      <c r="I6" s="4" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="11" t="n">
+      <c r="J6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="12" t="n">
+      <c r="K6" s="4" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="11" t="n">
+      <c r="L6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="12" t="n">
+      <c r="O6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="12" t="n">
+      <c r="P6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="3" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="4" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="12" t="e">
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="11" t="n">
+      <c r="N7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="12" t="n">
+      <c r="O7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="12" t="e">
+      <c r="P7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="12" t="e">
+      <c r="R7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="12" t="e">
+      <c r="T7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="10"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="2"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="3" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="4" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11" t="n">
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="12" t="n">
+      <c r="K9" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="12" t="e">
+      <c r="L9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="11" t="n">
+      <c r="N9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="12" t="e">
+      <c r="Q9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="11" t="n">
+      <c r="R9" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="12" t="e">
+      <c r="S9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="12" t="e">
+      <c r="T9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="3" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="2" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="10" t="e">
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10" t="e">
+      <c r="N10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="10" t="e">
+      <c r="R10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="10" t="e">
+      <c r="T10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
+      <c r="A16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="11" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
+      <c r="A19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1355,6 +1390,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create isDate function edit getDelayIf to use new isDate function rather than the lubridate version
</commit_message>
<xml_diff>
--- a/inst/extdata/excelfile.xlsx
+++ b/inst/extdata/excelfile.xlsx
@@ -308,6 +308,17 @@
       <b/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF65B32E"/>
+      <name val="Tahoma"/>
+      <b/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF00FF00"/>
       <name val="Calibri"/>
@@ -322,17 +333,6 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Symbol"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF65B32E"/>
-      <name val="Tahoma"/>
-      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -383,6 +383,17 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -401,17 +412,6 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -421,40 +421,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -785,31 +785,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -821,533 +821,533 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="3" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="3" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="3" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="4"/>
+      <c r="U2" s="9"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="13"/>
+      <c r="A3" s="5"/>
       <c r="B3" t="n">
         <v>67</v>
       </c>
       <c r="C3" t="n">
         <v>0.744444444444444</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="3" t="n">
         <f>SUM(D4,F4,H4,J4,L4,N4,P4,R4,T4)</f>
         <v>772</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="n">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="n">
         <v>145</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11" t="n">
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="n">
         <v>127</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="n">
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="n">
         <v>201</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11" t="n">
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11" t="n">
+      <c r="K4" s="2"/>
+      <c r="L4" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11" t="n">
+      <c r="M4" s="2"/>
+      <c r="N4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11" t="n">
+      <c r="O4" s="2"/>
+      <c r="P4" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="11" t="n">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S4" s="10"/>
-      <c r="T4" s="11" t="n">
+      <c r="S4" s="2"/>
+      <c r="T4" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U4" s="10"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="3" t="n">
         <f>SUM(D5,F5,H5,J5,L5,N5,P5,R5,T5)</f>
         <v>717</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="4" t="n">
         <f>B5/$B$4</f>
         <v>0.92875647668393779</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="3" t="n">
         <v>131</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="4" t="n">
         <v>0.90344827586206899</v>
       </c>
-      <c r="F5" s="11" t="n">
+      <c r="F5" s="3" t="n">
         <v>121</v>
       </c>
-      <c r="G5" s="12" t="n">
+      <c r="G5" s="4" t="n">
         <v>0.952755905511811</v>
       </c>
-      <c r="H5" s="11" t="n">
+      <c r="H5" s="3" t="n">
         <v>168</v>
       </c>
-      <c r="I5" s="12" t="n">
+      <c r="I5" s="4" t="n">
         <v>0.83582089552238803</v>
       </c>
-      <c r="J5" s="11" t="n">
+      <c r="J5" s="3" t="n">
         <v>99</v>
       </c>
-      <c r="K5" s="12" t="n">
+      <c r="K5" s="4" t="n">
         <v>0.98019801980198018</v>
       </c>
-      <c r="L5" s="11" t="n">
+      <c r="L5" s="3" t="n">
         <v>198</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="M5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="11" t="n">
+      <c r="N5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>226</v>
       </c>
-      <c r="Q5" s="12" t="n">
+      <c r="Q5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="R5" s="11" t="n">
+      <c r="R5" s="3" t="n">
         <v>304</v>
       </c>
-      <c r="S5" s="12" t="n">
+      <c r="S5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T5" s="11" t="n">
+      <c r="T5" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="U5" s="12" t="n">
+      <c r="U5" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="3" t="n">
         <f>SUM(D6,F6,H6,J6,L6,N6,P6,R6,T6)</f>
         <v>55</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="4" t="n">
         <f>B6/$B$4</f>
         <v>7.1243523316062179E-2</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="12" t="n">
+      <c r="E6" s="4" t="n">
         <v>9.6551724137931033E-2</v>
       </c>
-      <c r="F6" s="11" t="n">
+      <c r="F6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="12" t="n">
+      <c r="G6" s="4" t="n">
         <v>4.7244094488188976E-2</v>
       </c>
-      <c r="H6" s="11" t="n">
+      <c r="H6" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="12" t="n">
+      <c r="I6" s="4" t="n">
         <v>0.16417910447761194</v>
       </c>
-      <c r="J6" s="11" t="n">
+      <c r="J6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="12" t="n">
+      <c r="K6" s="4" t="n">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="11" t="n">
+      <c r="L6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="12" t="n">
+      <c r="O6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="12" t="n">
+      <c r="P6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="3" t="n">
         <f>SUM(D7,F7,H7,J7,L7,N7,P7,R7,T7)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="4" t="n">
         <f>B7/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="12" t="e">
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N7" s="11" t="n">
+      <c r="N7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="12" t="n">
+      <c r="O7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="12" t="e">
+      <c r="P7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="12" t="e">
+      <c r="R7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="12" t="e">
+      <c r="T7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="10"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="2"/>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="3" t="n">
         <f>SUM(D9,F9,H9,J9,L9,N9,P9,R9,T9)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="4" t="n">
         <f>B9/$B$6</f>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="D9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11" t="n">
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="12" t="n">
+      <c r="K9" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="12" t="e">
+      <c r="L9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="11" t="n">
+      <c r="N9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="Q9" s="12" t="e">
+      <c r="Q9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="11" t="n">
+      <c r="R9" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="S9" s="12" t="e">
+      <c r="S9" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="T9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="12" t="e">
+      <c r="T9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="3" t="n">
         <f>SUM(D10,F10,H10,J10,L10,N10,P10,R10,T10)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="2" t="n">
         <f>B10/$B$6</f>
         <v>0</v>
       </c>
-      <c r="D10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="10" t="e">
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10" t="e">
+      <c r="N10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="R10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="10" t="e">
+      <c r="R10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="10" t="e">
+      <c r="T10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
+      <c r="A16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="11" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
+      <c r="A19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>